<commit_message>
Modify temperature data form
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerator_temperature_data/forms/refrigerator_temperature_data/refrigerator_temperature_data.xlsx
+++ b/app/config/tables/refrigerator_temperature_data/forms/refrigerator_temperature_data/refrigerator_temperature_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11055" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="11052" yWindow="0" windowWidth="3396" windowHeight="1356" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="117">
   <si>
     <t>clause</t>
   </si>
@@ -274,9 +274,6 @@
     <t>birthdate</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>display.prompt.text.fr</t>
   </si>
   <si>
@@ -346,82 +343,40 @@
     <t>Datos de Temperatura del Refrigerador</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>average_temperature</t>
-  </si>
-  <si>
-    <t>lower_alarm_status</t>
-  </si>
-  <si>
-    <t>minimum_temperature</t>
-  </si>
-  <si>
-    <t>cumulative_duration_below_lower_limit</t>
-  </si>
-  <si>
-    <t>upper_alarm_status</t>
-  </si>
-  <si>
-    <t>maximum_temperature</t>
-  </si>
-  <si>
-    <t>cumulative_duration_above_upper_limit</t>
-  </si>
-  <si>
-    <t>Lower Alarm Status</t>
-  </si>
-  <si>
-    <t>Cumulative Duration Below Lower Limit</t>
-  </si>
-  <si>
-    <t>Upper Alarm Status</t>
-  </si>
-  <si>
-    <t>Cumulative Duration Above Upper Limit</t>
-  </si>
-  <si>
-    <t>Minimum Temperature</t>
-  </si>
-  <si>
-    <t>Maximum Temperature</t>
-  </si>
-  <si>
-    <t>(minutes)</t>
-  </si>
-  <si>
-    <t>(degrees Celsius)</t>
-  </si>
-  <si>
-    <t>(grados Celsius)</t>
-  </si>
-  <si>
-    <t>Average Temperature</t>
-  </si>
-  <si>
-    <t>Temperatura media</t>
-  </si>
-  <si>
-    <t>Estado de alarma inferior</t>
-  </si>
-  <si>
-    <t>Temperatura mínima</t>
-  </si>
-  <si>
-    <t>Duración acumulativa por debajo del límite inferior</t>
-  </si>
-  <si>
-    <t>Estado de alarma superior</t>
-  </si>
-  <si>
-    <t>Temperatura máxima</t>
-  </si>
-  <si>
-    <t>Duración acumulativa por encima del límite superior</t>
-  </si>
-  <si>
-    <t>(minutos)</t>
+    <t>number_of_high_alarms_30</t>
+  </si>
+  <si>
+    <t>number_of_low_alarms_30</t>
+  </si>
+  <si>
+    <t>days_temp_above_8_30</t>
+  </si>
+  <si>
+    <t>days_temp_below_2_30</t>
+  </si>
+  <si>
+    <t>Number of High Alarms Over Last 30 Days</t>
+  </si>
+  <si>
+    <t>Number of Low Alarms Over Last 30 Days</t>
+  </si>
+  <si>
+    <t>Days with Temperatures Above 8°C, Last 30 Days</t>
+  </si>
+  <si>
+    <t>Days with Temperature Below 2°C, Last 30 Days</t>
+  </si>
+  <si>
+    <t>Número de alarmas altas en los últimos 30 días</t>
+  </si>
+  <si>
+    <t>Número de alarmas bajas en los últimos 30 días</t>
+  </si>
+  <si>
+    <t>Días con temperaturas superiores a 8 ° C, últimos 30 días</t>
+  </si>
+  <si>
+    <t>Días con temperatura inferior a 2 ° C, últimos 30 días</t>
   </si>
 </sst>
 </file>
@@ -1045,16 +1000,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="23" customWidth="1"/>
-    <col min="2" max="2" width="8.75" style="23"/>
+    <col min="2" max="2" width="8.69921875" style="23"/>
     <col min="3" max="3" width="18" style="23" customWidth="1"/>
-    <col min="4" max="4" width="24.25" style="23" customWidth="1"/>
-    <col min="5" max="16384" width="8.75" style="23"/>
+    <col min="4" max="4" width="24.19921875" style="23" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1062,27 +1017,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1095,29 +1050,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="37.25" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="34.25" customWidth="1"/>
-    <col min="5" max="5" width="37.125" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="2" width="37.19921875" customWidth="1"/>
+    <col min="3" max="3" width="32.8984375" customWidth="1"/>
+    <col min="4" max="4" width="34.19921875" customWidth="1"/>
+    <col min="5" max="5" width="37.09765625" customWidth="1"/>
     <col min="6" max="6" width="51" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="43.875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="24.625" customWidth="1"/>
+    <col min="8" max="8" width="43.8984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="24.59765625" customWidth="1"/>
     <col min="10" max="10" width="39.5" customWidth="1"/>
     <col min="11" max="11" width="39.5" style="12" customWidth="1"/>
     <col min="12" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="13" width="24.75" customWidth="1"/>
+    <col min="13" max="13" width="24.69921875" customWidth="1"/>
     <col min="14" max="1027" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1095,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>68</v>
@@ -1149,7 +1104,7 @@
         <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1158,7 +1113,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -1173,7 +1128,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -1190,7 +1145,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1207,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -1219,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>65</v>
       </c>
@@ -1227,7 +1182,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1241,10 +1196,10 @@
         <v>74</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>81</v>
       </c>
@@ -1259,7 +1214,7 @@
         <v>78</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>80</v>
@@ -1272,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1284,176 +1239,129 @@
       <c r="H8" s="16"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C9" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
         <v>106</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" t="s">
-        <v>109</v>
-      </c>
       <c r="F11" s="16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" s="21" t="s">
         <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="21"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="21"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="21"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F20" s="24"/>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="6:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F21" s="13"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F22" s="25"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D34" s="12"/>
       <c r="F34" s="13"/>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D35" s="12"/>
       <c r="F35" s="13"/>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F36" s="25"/>
       <c r="H36" s="17"/>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D49" s="12"/>
       <c r="F49" s="25"/>
       <c r="H49" s="25"/>
     </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D50" s="12"/>
       <c r="F50" s="13"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F51" s="25"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="79" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
@@ -1462,7 +1370,7 @@
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
     </row>
-    <row r="80" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -1472,7 +1380,7 @@
       <c r="G80" s="19"/>
       <c r="H80" s="19"/>
     </row>
-    <row r="82" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1487,14 +1395,14 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.75" customWidth="1"/>
-    <col min="2" max="2" width="71.125" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
+    <col min="2" max="2" width="71.09765625" customWidth="1"/>
     <col min="7" max="7" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -1502,12 +1410,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
     </row>
   </sheetData>
@@ -1523,12 +1431,12 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.625" customWidth="1"/>
+    <col min="2" max="2" width="28.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1447,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1553,17 +1461,17 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.375" customWidth="1"/>
+    <col min="1" max="1" width="35.3984375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="42.625" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="42.59765625" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1577,116 +1485,116 @@
         <v>6</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D2" s="10"/>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E3" s="20"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" s="12"/>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" s="12"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E8" s="22"/>
     </row>
-    <row r="10" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="22"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E12" s="22"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E15" s="20"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="20"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="E19" s="20"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="C20" s="12"/>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="C21" s="12"/>
       <c r="E21" s="20"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="C22" s="12"/>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="C23" s="12"/>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="C24" s="12"/>
       <c r="E24" s="20"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="20"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="C29" s="12"/>
       <c r="E29" s="20"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="C30" s="12"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="C31" s="12"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="C32" s="12"/>
       <c r="E32" s="20"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="23"/>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
       <c r="E34" s="23"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="23"/>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -1706,20 +1614,20 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="47.125" customWidth="1"/>
-    <col min="8" max="8" width="38.875" customWidth="1"/>
+    <col min="7" max="7" width="47.09765625" customWidth="1"/>
+    <col min="8" max="8" width="38.8984375" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1760,24 +1668,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.125" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="23.3984375" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.09765625" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="23.625" customWidth="1"/>
+    <col min="8" max="8" width="23.59765625" customWidth="1"/>
     <col min="9" max="1026" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1791,7 +1699,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>29</v>
@@ -1800,38 +1708,38 @@
         <v>30</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1839,7 +1747,7 @@
         <v>20191213</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1847,7 +1755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1858,10 +1766,10 @@
         <v>38</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1872,21 +1780,21 @@
         <v>41</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
         <v>89</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>90</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>91</v>
-      </c>
-      <c r="H9" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1908,16 +1816,16 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1934,7 +1842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
@@ -1951,7 +1859,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>45</v>
       </c>
@@ -1965,10 +1873,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>45</v>
       </c>
@@ -1982,10 +1890,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -2002,7 +1910,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -2019,7 +1927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
@@ -2036,7 +1944,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>

</xml_diff>